<commit_message>
[23 2] update excel_zad2.py
</commit_message>
<xml_diff>
--- a/day23_28_02_2026/xlsxwriter5.xlsx
+++ b/day23_28_02_2026/xlsxwriter5.xlsx
@@ -7,15 +7,33 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Witaj1</t>
+  </si>
+  <si>
+    <t>Witaj  2</t>
+  </si>
+  <si>
+    <t>Witaj 3</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
+    <numFmt numFmtId="165" formatCode="[$-409]0.00"/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -23,16 +41,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -40,12 +72,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -340,12 +392,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="2">
+        <v>42656</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="3">
+        <v>3.333333</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6">
+        <f>SUM(A4, 2)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[23 4] update excel_zad2.py
</commit_message>
<xml_diff>
--- a/day23_28_02_2026/xlsxwriter5.xlsx
+++ b/day23_28_02_2026/xlsxwriter5.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Witaj1</t>
   </si>
@@ -23,6 +23,12 @@
   </si>
   <si>
     <t>Witaj 3</t>
+  </si>
+  <si>
+    <t>Styczeń</t>
+  </si>
+  <si>
+    <t>Luty</t>
   </si>
 </sst>
 </file>
@@ -105,6 +111,227 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Sprzedaż</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Arkusz1!A30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Arkusz1!B20:C20</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Styczeń</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Luty</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz1!B21:C21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>150</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="50010001"/>
+        <c:axId val="50010002"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="50010001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>OS X</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50010002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50010002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>OS Y</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50010001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="django_komendy.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3048000" y="0"/>
+          <a:ext cx="8172450" cy="3838575"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -392,7 +619,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -429,7 +656,24 @@
         <v>0</v>
       </c>
     </row>
+    <row r="20" spans="2:3">
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3">
+      <c r="B21">
+        <v>100</v>
+      </c>
+      <c r="C21">
+        <v>150</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>